<commit_message>
@MatheusHenrique005 Atualizando tabela de alertas
</commit_message>
<xml_diff>
--- a/massa de dados/massa_de_dados.xlsx
+++ b/massa de dados/massa_de_dados.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c6a82778d5878752/Área de Trabalho/cervejaria_arquiComp/massa de dados/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/492d2352ca998f5d/Documentos/GitHub/cervejaria_arquiComp/massa de dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D2651A15-53BD-492A-B856-677F7087020E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="264" documentId="8_{D2651A15-53BD-492A-B856-677F7087020E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B05AA08-80B4-4854-85B4-0CE425AB39A4}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{E6F3F1C6-B4A2-40BA-B483-A3A0619A04BD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{E6F3F1C6-B4A2-40BA-B483-A3A0619A04BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
   <si>
     <t>Arduino</t>
   </si>
@@ -69,6 +70,96 @@
   </si>
   <si>
     <t>Simulado em Graus Celsius (°C)</t>
+  </si>
+  <si>
+    <t>a - maceração</t>
+  </si>
+  <si>
+    <t>b - maceração</t>
+  </si>
+  <si>
+    <t>a - malteração1</t>
+  </si>
+  <si>
+    <t>b - malteração2</t>
+  </si>
+  <si>
+    <t>a - malteração2</t>
+  </si>
+  <si>
+    <t>b - malteração1</t>
+  </si>
+  <si>
+    <t>a - malteração3</t>
+  </si>
+  <si>
+    <t>b - malteração3</t>
+  </si>
+  <si>
+    <t>a - moagem</t>
+  </si>
+  <si>
+    <t>b - moagem</t>
+  </si>
+  <si>
+    <t>a - brassagem1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> b - brassagem1</t>
+  </si>
+  <si>
+    <t>a - brassagem2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> b - brassagem2</t>
+  </si>
+  <si>
+    <t>a - brassagem3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> b - brassagem3</t>
+  </si>
+  <si>
+    <t>a - fervura</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> b - fervura</t>
+  </si>
+  <si>
+    <t>a - resfriamento1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> b - resfriamento2</t>
+  </si>
+  <si>
+    <t>a - resfriamento2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> b - resfriamento1</t>
+  </si>
+  <si>
+    <t>a - resfriamento3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> b - resfriamento3</t>
+  </si>
+  <si>
+    <t>a - maturação</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> b - maturação</t>
+  </si>
+  <si>
+    <t>a - pasteurização</t>
+  </si>
+  <si>
+    <t>b - pasteurização</t>
+  </si>
+  <si>
+    <t>a - produto final</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> b - produto final</t>
   </si>
 </sst>
 </file>
@@ -131,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -142,6 +233,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -157,6 +253,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -458,18 +558,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{042C62C4-BA87-4AC6-999D-A18066E7FD64}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -478,19 +578,19 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3">
         <v>26</v>
       </c>
-      <c r="C2" s="3">
-        <f>B2-12</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C2" s="4">
+        <f xml:space="preserve"> 15 - (1.23/26)</f>
+        <v>14.952692307692308</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -502,7 +602,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -514,7 +614,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -526,7 +626,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -538,7 +638,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -550,7 +650,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -562,7 +662,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -574,7 +674,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
@@ -586,7 +686,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
@@ -598,7 +698,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
@@ -610,7 +710,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
@@ -622,7 +722,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
@@ -634,7 +734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
@@ -646,7 +746,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
@@ -662,4 +762,486 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25AC6C9D-9B7F-411E-884F-76B2D7C4F56C}">
+  <dimension ref="C3:N61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C4" s="5">
+        <f xml:space="preserve"> (15-12)/(27.77-25.33)</f>
+        <v>1.2295081967213108</v>
+      </c>
+      <c r="D4" s="5">
+        <f xml:space="preserve"> 12 - (C4/25.33)</f>
+        <v>11.951460394918227</v>
+      </c>
+    </row>
+    <row r="5" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C5" s="5">
+        <f xml:space="preserve"> (15-12)/2.44</f>
+        <v>1.2295081967213115</v>
+      </c>
+      <c r="D5" s="5">
+        <f xml:space="preserve"> 15 - (C5/27.77)</f>
+        <v>14.955725308004274</v>
+      </c>
+    </row>
+    <row r="6" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C8" s="5">
+        <f xml:space="preserve"> (50 - 48)/(27.77-25.33)</f>
+        <v>0.81967213114754056</v>
+      </c>
+      <c r="D8" s="5">
+        <f xml:space="preserve"> 48 - (C8/25.33)</f>
+        <v>47.967640263278817</v>
+      </c>
+      <c r="N8" s="6"/>
+    </row>
+    <row r="9" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C9" s="5">
+        <f xml:space="preserve"> (50 - 48)/(27.77-25.33)</f>
+        <v>0.81967213114754056</v>
+      </c>
+      <c r="D9" s="5">
+        <f xml:space="preserve"> 50 - (C9/27.77)</f>
+        <v>49.970483538669519</v>
+      </c>
+    </row>
+    <row r="10" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C12" s="5">
+        <f xml:space="preserve"> (75 - 70)/(27.77-25.33)</f>
+        <v>2.0491803278688514</v>
+      </c>
+      <c r="D12" s="5">
+        <f xml:space="preserve"> 70 - (C12/25.33)</f>
+        <v>69.919100658197038</v>
+      </c>
+    </row>
+    <row r="13" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C13" s="5">
+        <f xml:space="preserve"> (75 - 70)/(27.77-25.33)</f>
+        <v>2.0491803278688514</v>
+      </c>
+      <c r="D13" s="5">
+        <f xml:space="preserve"> 75 - (C13/27.77)</f>
+        <v>74.926208846673788</v>
+      </c>
+    </row>
+    <row r="14" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C16" s="5">
+        <f xml:space="preserve"> (90 - 75)/(27.77-25.33)</f>
+        <v>6.1475409836065538</v>
+      </c>
+      <c r="D16" s="5">
+        <f xml:space="preserve"> 75 - (C16/25.33)</f>
+        <v>74.75730197459113</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="5">
+        <f xml:space="preserve"> (90 - 75)/(27.77-25.33)</f>
+        <v>6.1475409836065538</v>
+      </c>
+      <c r="D17" s="5">
+        <f xml:space="preserve"> 90 - (C17/27.77)</f>
+        <v>89.778626540021364</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="5"/>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="5">
+        <f xml:space="preserve"> (72 - 62)/(27.77-25.33)</f>
+        <v>4.0983606557377028</v>
+      </c>
+      <c r="D20" s="5">
+        <f xml:space="preserve"> 62 - (C20/25.33)</f>
+        <v>61.838201316394091</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C21" s="5">
+        <f xml:space="preserve"> (72 - 62)/(27.77-25.33)</f>
+        <v>4.0983606557377028</v>
+      </c>
+      <c r="D21" s="5">
+        <f xml:space="preserve"> 72 - (C21/27.77)</f>
+        <v>71.852417693347576</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="5"/>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C24" s="5">
+        <f xml:space="preserve"> (40 - 35)/(27.77-25.33)</f>
+        <v>2.0491803278688514</v>
+      </c>
+      <c r="D24" s="5">
+        <f xml:space="preserve"> 35 - (C24/25.33)</f>
+        <v>34.919100658197046</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C25" s="5">
+        <f xml:space="preserve"> (40 - 35)/(27.77-25.33)</f>
+        <v>2.0491803278688514</v>
+      </c>
+      <c r="D25" s="5">
+        <f xml:space="preserve"> 40 - (C25/27.77)</f>
+        <v>39.926208846673788</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D26" s="5"/>
+    </row>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C28" s="5">
+        <f xml:space="preserve"> (70 - 55)/(27.77-25.33)</f>
+        <v>6.1475409836065538</v>
+      </c>
+      <c r="D28" s="5">
+        <f xml:space="preserve"> 55 - (C28/25.33)</f>
+        <v>54.757301974591137</v>
+      </c>
+    </row>
+    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C29" s="5">
+        <f xml:space="preserve"> (70 - 55)/(27.77-25.33)</f>
+        <v>6.1475409836065538</v>
+      </c>
+      <c r="D29" s="5">
+        <f xml:space="preserve"> 70 - (C29/27.77)</f>
+        <v>69.778626540021364</v>
+      </c>
+    </row>
+    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="5"/>
+    </row>
+    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C32" s="5">
+        <f xml:space="preserve"> (67 - 62)/(27.77-25.33)</f>
+        <v>2.0491803278688514</v>
+      </c>
+      <c r="D32" s="5">
+        <f xml:space="preserve"> 62 - (C32/25.33)</f>
+        <v>61.919100658197046</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33" s="5">
+        <f xml:space="preserve"> (67 - 62)/(27.77-25.33)</f>
+        <v>2.0491803278688514</v>
+      </c>
+      <c r="D33" s="5">
+        <f xml:space="preserve"> 67 - (C33/27.77)</f>
+        <v>66.926208846673788</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="5"/>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C36" s="5">
+        <f xml:space="preserve"> (102 - 100)/(27.77-25.33)</f>
+        <v>0.81967213114754056</v>
+      </c>
+      <c r="D36" s="5">
+        <f xml:space="preserve"> 100 - (C36/25.33)</f>
+        <v>99.967640263278824</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C37" s="5">
+        <f xml:space="preserve"> (102 - 100)/(27.77-25.33)</f>
+        <v>0.81967213114754056</v>
+      </c>
+      <c r="D37" s="5">
+        <f xml:space="preserve"> 102 - (C37/27.77)</f>
+        <v>101.97048353866951</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="5"/>
+    </row>
+    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>29</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C40" s="5">
+        <f xml:space="preserve"> (12 - 7)/(27.77-25.33)</f>
+        <v>2.0491803278688514</v>
+      </c>
+      <c r="D40" s="5">
+        <f xml:space="preserve"> 7 - (C40/25.33)</f>
+        <v>6.9191006581970447</v>
+      </c>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C41" s="5">
+        <f xml:space="preserve"> (12 - 7)/(27.77-25.33)</f>
+        <v>2.0491803278688514</v>
+      </c>
+      <c r="D41" s="5">
+        <f xml:space="preserve"> 12 - (C41/27.77)</f>
+        <v>11.92620884667379</v>
+      </c>
+    </row>
+    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D42" s="5"/>
+    </row>
+    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>31</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C44" s="5">
+        <f xml:space="preserve"> (17 - 12)/(27.77-25.33)</f>
+        <v>2.0491803278688514</v>
+      </c>
+      <c r="D44" s="5">
+        <f xml:space="preserve">  12 - (C44/25.33)</f>
+        <v>11.919100658197046</v>
+      </c>
+    </row>
+    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C45" s="5">
+        <f xml:space="preserve"> (17 - 12)/(27.77-25.33)</f>
+        <v>2.0491803278688514</v>
+      </c>
+      <c r="D45" s="5">
+        <f xml:space="preserve"> 17 - (C45/27.77)</f>
+        <v>16.926208846673791</v>
+      </c>
+    </row>
+    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D46" s="5"/>
+    </row>
+    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>33</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C48" s="5">
+        <f xml:space="preserve"> (6 - 4)/(27.77-25.33)</f>
+        <v>0.81967213114754056</v>
+      </c>
+      <c r="D48" s="5">
+        <f xml:space="preserve">  4 - (C48/25.33)</f>
+        <v>3.9676402632788181</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C49" s="5">
+        <f xml:space="preserve"> (6 - 4)/(27.77-25.33)</f>
+        <v>0.81967213114754056</v>
+      </c>
+      <c r="D49" s="5">
+        <f xml:space="preserve"> 6 - (C49/27.77)</f>
+        <v>5.9704835386695159</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D50" s="5"/>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>35</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C52" s="5">
+        <f xml:space="preserve"> (2 - 0)/(27.77-25.33)</f>
+        <v>0.81967213114754056</v>
+      </c>
+      <c r="D52" s="5">
+        <f xml:space="preserve">  0 - (C52/25.33)</f>
+        <v>-3.2359736721182024E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C53" s="5">
+        <f xml:space="preserve"> (2 - 0)/(27.77-25.33)</f>
+        <v>0.81967213114754056</v>
+      </c>
+      <c r="D53" s="5">
+        <f xml:space="preserve"> 2 - (C53/27.77)</f>
+        <v>1.9704835386695161</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D54" s="5"/>
+    </row>
+    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>37</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C56" s="5">
+        <f xml:space="preserve"> (70 - 60)/(27.77-25.33)</f>
+        <v>4.0983606557377028</v>
+      </c>
+      <c r="D56" s="5">
+        <f xml:space="preserve">  60 - (C56/25.33)</f>
+        <v>59.838201316394091</v>
+      </c>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C57" s="5">
+        <f xml:space="preserve"> (70 - 60)/(27.77-25.33)</f>
+        <v>4.0983606557377028</v>
+      </c>
+      <c r="D57" s="5">
+        <f xml:space="preserve"> 70 - (C57/27.77)</f>
+        <v>69.852417693347576</v>
+      </c>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D58" s="5"/>
+    </row>
+    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>39</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C60" s="5">
+        <f xml:space="preserve"> (7 - 2)/(27.77-25.33)</f>
+        <v>2.0491803278688514</v>
+      </c>
+      <c r="D60" s="5">
+        <f xml:space="preserve">  7 - (C60/25.33)</f>
+        <v>6.9191006581970447</v>
+      </c>
+    </row>
+    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C61" s="5">
+        <f xml:space="preserve"> (7 - 2)/(27.77-25.33)</f>
+        <v>2.0491803278688514</v>
+      </c>
+      <c r="D61" s="5">
+        <f xml:space="preserve"> 2 - (C61/27.77)</f>
+        <v>1.9262088466737901</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>